<commit_message>
finished visualizations; updated models
</commit_message>
<xml_diff>
--- a/models/table_2.xlsx
+++ b/models/table_2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="159">
   <si>
     <t xml:space="preserve">                       </t>
   </si>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">PanelOLS        </t>
   </si>
   <si>
-    <t xml:space="preserve">1759            </t>
+    <t xml:space="preserve">1768            </t>
   </si>
   <si>
     <t xml:space="preserve">Clustered       </t>
@@ -118,346 +118,352 @@
     <t xml:space="preserve">0.2397          </t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0572         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0153          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">136.84          </t>
+    <t xml:space="preserve">-0.1032         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0109          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">137.47          </t>
   </si>
   <si>
     <t xml:space="preserve">0.0000          </t>
   </si>
   <si>
-    <t xml:space="preserve">0.0453***       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0054)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1069*         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0574)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0653         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0682)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1634*        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0977)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3330**        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.1455)        </t>
+    <t xml:space="preserve">0.0423***       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0051)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1067*         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0573)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0656         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0683)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1671*        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0992)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3326**        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.1448)        </t>
   </si>
   <si>
     <t xml:space="preserve">                </t>
   </si>
   <si>
-    <t xml:space="preserve">0.2456          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0649         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0105          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">94.065          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0459***       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1057*         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0560)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0687)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1560         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0954)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3360**        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.1402)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0324**       </t>
+    <t xml:space="preserve">0.2455          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1132         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0060          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">94.478          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0428***       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0050)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1055*         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0559)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0657         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0688)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1596*        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0969)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3357**        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.1395)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0323**       </t>
   </si>
   <si>
     <t xml:space="preserve">(0.0134)        </t>
   </si>
   <si>
-    <t xml:space="preserve">0.0272**        </t>
+    <t xml:space="preserve">0.0271**        </t>
   </si>
   <si>
     <t xml:space="preserve">(0.0135)        </t>
   </si>
   <si>
-    <t xml:space="preserve">0.5347          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8243          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7681          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">248.80          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0411***       </t>
+    <t xml:space="preserve">0.5339          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8143          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7666          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">249.16          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0397***       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0025)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0654**        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0282)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0565         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0436)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0717         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0486)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1194          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0942)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0115         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0081)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0080          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0087)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5873***       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0842)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0265          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0270)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5508          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7333          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7036          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">236.91          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0390***       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0028)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0316          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0308)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0724         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0457)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1033*        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0535)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0803          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.1050)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0070         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0068)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0094          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0089)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5357***       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0881)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0104         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0212)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1289***       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0432)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5432          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7715          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7343          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">229.79          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0391***       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0026)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0437          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0306)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0517         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0437)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0890*        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0516)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0950          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0966)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0088         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0075)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0071          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0091)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5593***       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0906)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0067          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0234)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0734**        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0349)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5471          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7523          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7190          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">233.43          </t>
   </si>
   <si>
     <t xml:space="preserve">(0.0027)        </t>
   </si>
   <si>
-    <t xml:space="preserve">0.0656**        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0283)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0566         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0434)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0699         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0476)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1192          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0945)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0117         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0082)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0081          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0087)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5886***       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0841)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0263          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0275)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5516          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7376          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7048          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">236.60          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0403***       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0031)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0316          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0308)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0720         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0455)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1010*        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0524)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0803          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.1056)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0070         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0068)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0094          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0089)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5364***       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0884)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0103         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0221)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1280***       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0428)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5441          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7789          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7356          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">229.52          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0404***       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0028)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0438          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0306)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0519         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0435)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0872*        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0506)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0948          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0973)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0088         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0076)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0070          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0091)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5602***       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0908)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0073          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0244)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0730**        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0347)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5480          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7582          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7203          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">233.14          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0029)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0369          </t>
+    <t xml:space="preserve">0.0368          </t>
   </si>
   <si>
     <t xml:space="preserve">(0.0310)        </t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0594         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0442)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0943*        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0517)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0867          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.1008)        </t>
+    <t xml:space="preserve">-0.0595         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0444)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0963*        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0528)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0868          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.1002)        </t>
   </si>
   <si>
     <t xml:space="preserve">-0.0078         </t>
@@ -469,22 +475,22 @@
     <t xml:space="preserve">0.0079          </t>
   </si>
   <si>
-    <t xml:space="preserve">0.5480***       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0907)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0015         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0233)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1018**        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0402)        </t>
+    <t xml:space="preserve">0.5472***       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0904)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0020         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0222)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1024**        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0405)        </t>
   </si>
 </sst>
 </file>
@@ -974,16 +980,16 @@
         <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -997,16 +1003,16 @@
         <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F7" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1020,16 +1026,16 @@
         <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1043,16 +1049,16 @@
         <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1066,16 +1072,16 @@
         <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1112,16 +1118,16 @@
         <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F12" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1132,19 +1138,19 @@
         <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G13" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1155,19 +1161,19 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F14" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G14" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1178,19 +1184,19 @@
         <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F15" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G15" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1201,19 +1207,19 @@
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F16" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G16" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1224,19 +1230,19 @@
         <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F17" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G17" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1247,19 +1253,19 @@
         <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G18" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1270,19 +1276,19 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F19" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1293,19 +1299,19 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F20" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G20" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1316,19 +1322,19 @@
         <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F21" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G21" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1339,19 +1345,19 @@
         <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F22" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G22" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1362,19 +1368,19 @@
         <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G23" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1385,19 +1391,19 @@
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F24" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G24" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1408,19 +1414,19 @@
         <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F25" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G25" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1434,16 +1440,16 @@
         <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F26" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G26" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1457,16 +1463,16 @@
         <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E27" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F27" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G27" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1480,16 +1486,16 @@
         <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F28" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G28" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1503,16 +1509,16 @@
         <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E29" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F29" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G29" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1529,7 +1535,7 @@
         <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F30" t="s">
         <v>48</v>
@@ -1552,7 +1558,7 @@
         <v>48</v>
       </c>
       <c r="E31" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F31" t="s">
         <v>48</v>
@@ -1578,7 +1584,7 @@
         <v>48</v>
       </c>
       <c r="F32" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G32" t="s">
         <v>48</v>
@@ -1601,7 +1607,7 @@
         <v>48</v>
       </c>
       <c r="F33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G33" t="s">
         <v>48</v>
@@ -1627,7 +1633,7 @@
         <v>48</v>
       </c>
       <c r="G34" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1650,7 +1656,7 @@
         <v>48</v>
       </c>
       <c r="G35" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>